<commit_message>
added excel file importing  for classes modules and semaines
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC45D4F-2A94-4601-903E-ECEFB24A6D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,32 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Classe</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Java</t>
   </si>
   <si>
-    <t>maryem@gmail.com</t>
-  </si>
-  <si>
     <t>T.I</t>
   </si>
   <si>
-    <t>boustani@gmail.com</t>
-  </si>
-  <si>
-    <t>4.Ginfo\4GTR</t>
-  </si>
-  <si>
     <t>R.O</t>
   </si>
   <si>
@@ -49,25 +32,46 @@
     <t>4.Ginfo</t>
   </si>
   <si>
-    <t>4.GInfo\4GTR</t>
-  </si>
-  <si>
     <t>3.GInfo</t>
   </si>
   <si>
     <t>Analyse 3</t>
   </si>
   <si>
-    <t>ammar@gmail.com</t>
-  </si>
-  <si>
     <t>Cp 2</t>
+  </si>
+  <si>
+    <t>NomModule</t>
+  </si>
+  <si>
+    <t>Ensiegnant_Email</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>profmail1@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail2@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail3@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail4@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail5@gmail.com</t>
+  </si>
+  <si>
+    <t>4.Ginfo/4GTR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,7 +115,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -128,7 +132,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -203,6 +207,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -238,6 +259,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,92 +451,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{FC419558-7EDC-45D9-9777-09E464F9D86D}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{846CD298-4027-449D-80CE-5099F18E216D}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{54C20351-5D66-45F3-A3AA-8AA905AD046A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the logic into its modal
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,32 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
-  <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Classe</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Java</t>
   </si>
   <si>
-    <t>maryem@gmail.com</t>
-  </si>
-  <si>
     <t>T.I</t>
   </si>
   <si>
-    <t>boustani@gmail.com</t>
-  </si>
-  <si>
-    <t>4.Ginfo\4GTR</t>
-  </si>
-  <si>
     <t>R.O</t>
   </si>
   <si>
@@ -49,19 +31,40 @@
     <t>4.Ginfo</t>
   </si>
   <si>
-    <t>4.GInfo\4GTR</t>
-  </si>
-  <si>
     <t>3.GInfo</t>
   </si>
   <si>
     <t>Analyse 3</t>
   </si>
   <si>
-    <t>ammar@gmail.com</t>
-  </si>
-  <si>
     <t>Cp 2</t>
+  </si>
+  <si>
+    <t>NomModule</t>
+  </si>
+  <si>
+    <t>Ensiegnant_Email</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>profmail1@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail2@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail3@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail4@gmail.com</t>
+  </si>
+  <si>
+    <t>profmail5@gmail.com</t>
+  </si>
+  <si>
+    <t>4.Ginfo/4.GTR</t>
   </si>
 </sst>
 </file>
@@ -417,88 +420,88 @@
   <dimension ref="D2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId3"/>
+    <hyperlink ref="E7" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added import deances with excel functionality
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC45D4F-2A94-4601-903E-ECEFB24A6D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C77F88-B783-4A8F-95E8-6DC85D5DF0EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
     <t>profmail5@gmail.com</t>
   </si>
   <si>
-    <t>4.Ginfo/4GTR</t>
+    <t>4.Ginfo/4.GTR</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="D2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed blank row in excel files
</commit_message>
<xml_diff>
--- a/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
+++ b/GestionDesAbsencesMigration/Excel files/importerModule.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBE09C68-B920-464E-B4BC-B87A1F719135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>T.I</t>
   </si>
@@ -38,12 +39,18 @@
   </si>
   <si>
     <t>profmail1@gmail.com</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>profmail3@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,7 +94,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -104,7 +111,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -179,6 +186,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -214,6 +238,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,14 +430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D3:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
@@ -437,15 +478,24 @@
       </c>
     </row>
     <row r="6" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E6" s="1"/>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E6" r:id="rId3" xr:uid="{D47A9B8C-5172-4726-9CD7-C3CC7B212543}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>